<commit_message>
debug data_input and model
</commit_message>
<xml_diff>
--- a/dieterpy/templates/basicmodeldata/data_input.xlsx
+++ b/dieterpy/templates/basicmodeldata/data_input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="741" activeTab="6"/>
+    <workbookView windowWidth="23040" windowHeight="9144" tabRatio="741" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="LICENSE" sheetId="1" r:id="rId1"/>
@@ -2322,7 +2322,7 @@
     <t>tech</t>
   </si>
   <si>
-    <t>Technologies</t>
+    <t>technologies</t>
   </si>
   <si>
     <t>B6</t>
@@ -2795,12 +2795,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="0.000"/>
-    <numFmt numFmtId="177" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="176" formatCode="mmm\-yy"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="0.000"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -2864,44 +2864,66 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2915,39 +2937,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2962,20 +2952,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2983,17 +2959,41 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3058,7 +3058,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3070,61 +3178,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3136,19 +3196,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3166,73 +3220,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3297,17 +3297,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3328,16 +3346,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3351,20 +3369,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3379,157 +3394,142 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3558,7 +3558,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="48" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3580,10 +3580,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3609,7 +3609,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3623,17 +3623,17 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3666,7 +3666,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3699,7 +3699,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -11153,8 +11153,8 @@
   <sheetPr/>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="I42" sqref="I42"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="5"/>
@@ -29077,7 +29077,7 @@
   <sheetPr/>
   <dimension ref="A1:AMJ89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>

</xml_diff>